<commit_message>
add results cross project
</commit_message>
<xml_diff>
--- a/Tools-Metrics Mapping.xlsx
+++ b/Tools-Metrics Mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuni-my.sharepoint.com/personal/dario_amorosodaragona_tuni_fi/Documents/TEST PREDITCION/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valeriapontillo/Desktop/ML-Test-Smell-Detection-Online-Appendix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{08F8A8B4-1F36-E440-AEB2-5E7F809A7D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1C0BC93-AF25-B04D-ADA9-C5B1FAE90338}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD8CF83-A450-7647-B991-68B6C1225983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1880" yWindow="1760" windowWidth="27640" windowHeight="16940" xr2:uid="{3BE1FC2A-C7FB-FD4B-A4B3-80D9545251F6}"/>
+    <workbookView xWindow="1160" yWindow="500" windowWidth="27640" windowHeight="16040" xr2:uid="{3BE1FC2A-C7FB-FD4B-A4B3-80D9545251F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -92,11 +92,6 @@
     <t>Taste [6]</t>
   </si>
   <si>
-    <t xml:space="preserve">Number os Production Types Method Invocations (PTMI) 
-Probability of a Class to be affected by Eager Test baisng on its textual content (PET)
-</t>
-  </si>
-  <si>
     <t>TEREDETECT [7]</t>
   </si>
   <si>
@@ -201,6 +196,11 @@
   <si>
     <t xml:space="preserve">Pair Redundancy is the ratio of covered items by one test artifact with respect to another one (PR)
 Suite Redundancy, is the ratio of covered items by one test with respect all others tests in the test suite (SR)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average Textual similarity between all the pairs methods called by the test method (TMC)
+Probability of a Class to be affected by Eager Test baisng on its textual content (PET)
 </t>
   </si>
 </sst>
@@ -370,7 +370,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -462,7 +462,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -760,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{751EA78D-691A-BD4E-A3EA-78CDDBD16B19}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -861,7 +861,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -869,76 +869,76 @@
     </row>
     <row r="8" spans="1:5" ht="51">
       <c r="A8" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
       <c r="E8" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="48">
       <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="18" t="s">
         <v>20</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="48">
       <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>22</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="48">
       <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="18" t="s">
         <v>24</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="96">
       <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="18" t="s">
         <v>26</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="64">
       <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="18" t="s">
         <v>28</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>29</v>
       </c>
       <c r="C15" s="17"/>
     </row>
     <row r="16" spans="1:5" ht="48">
       <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>30</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>31</v>
       </c>
       <c r="D16" s="19"/>
     </row>
     <row r="17" spans="1:2" ht="32">
       <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="18" t="s">
         <v>32</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:2" s="4" customFormat="1"/>

</xml_diff>